<commit_message>
Note that Health Cloud license is optional.
</commit_message>
<xml_diff>
--- a/Docs/CTT Package Installation Guide.xlsx
+++ b/Docs/CTT Package Installation Guide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="799" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="799" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pre Deployment Steps OLD" sheetId="13" state="hidden" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="240">
   <si>
     <t>Step #</t>
   </si>
@@ -1825,6 +1825,12 @@
 Salesforce Shield encryption is reccomended to protect PII information.
 ***NOTE FOR TA/SA***
 If you are starting from a fresh/greenfield Salesfore instance. It is recommended that you perform this step [STEP 1] in Production so that future Sandboxes would include the changes. PLEASE USE YOUR OWN DISCRETION ON THIS STEP</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>This is optional. As of 11/27/2020, the Health Cloud licenses are not in use in CTT.</t>
   </si>
 </sst>
 </file>
@@ -3031,7 +3037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3172,35 +3178,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="8" customWidth="1"/>
     <col min="2" max="2" width="85.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="C2" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -5758,9 +5771,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5935,27 +5951,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{163BEE74-E426-4F2E-930B-3665AF3B22A9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F46E04-9716-47DF-BE4E-10DD5FD22D24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="44c172eb-110d-4902-bcaf-f6375353b947"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="566fb1d1-6d97-4bc6-86b4-e8923ec84cbf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5980,9 +5984,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F46E04-9716-47DF-BE4E-10DD5FD22D24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{163BEE74-E426-4F2E-930B-3665AF3B22A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="44c172eb-110d-4902-bcaf-f6375353b947"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="566fb1d1-6d97-4bc6-86b4-e8923ec84cbf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>